<commit_message>
update excel parser to find end of time series automatically and add annotations as types
</commit_message>
<xml_diff>
--- a/tests/xls_pipeline_test/input/mapping/tensile_test_mapping.xlsx
+++ b/tests/xls_pipeline_test/input/mapping/tensile_test_mapping.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>key</t>
   </si>
@@ -34,9 +34,6 @@
     <t>time_series_start</t>
   </si>
   <si>
-    <t>time_series_end</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>https://w3id.org/steel/ProcessOntology/TestTime</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>A14</t>
   </si>
   <si>
@@ -193,9 +187,6 @@
     <t>A15</t>
   </si>
   <si>
-    <t>A474</t>
-  </si>
-  <si>
     <t>Standardkraft</t>
   </si>
   <si>
@@ -208,9 +199,6 @@
     <t>C15</t>
   </si>
   <si>
-    <t>C474</t>
-  </si>
-  <si>
     <t>Traversenweg absolut</t>
   </si>
   <si>
@@ -223,9 +211,6 @@
     <t>B15</t>
   </si>
   <si>
-    <t>B474</t>
-  </si>
-  <si>
     <t>Standardweg</t>
   </si>
   <si>
@@ -238,9 +223,6 @@
     <t>D15</t>
   </si>
   <si>
-    <t>D474</t>
-  </si>
-  <si>
     <t>Breitenänderung</t>
   </si>
   <si>
@@ -253,9 +235,6 @@
     <t>E15</t>
   </si>
   <si>
-    <t>E474</t>
-  </si>
-  <si>
     <t>Dehnung</t>
   </si>
   <si>
@@ -263,9 +242,6 @@
   </si>
   <si>
     <t>Q15</t>
-  </si>
-  <si>
-    <t>Q474</t>
   </si>
   <si>
     <t>÷</t>
@@ -326,15 +302,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -642,21 +615,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="62.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="64.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="62.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="64.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -681,409 +653,371 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>69</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>74</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>79</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I20" s="2"/>
+        <v>76</v>
+      </c>
+      <c r="H20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>